<commit_message>
Fixing issues with experiments validation
</commit_message>
<xml_diff>
--- a/src/assets/atac-seq.xlsx
+++ b/src/assets/atac-seq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AEEB6B-CA64-0B49-9C3F-127D9FDD21A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD579C-1CEF-B546-9FEA-1D214A7DD693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="278">
   <si>
     <t>Sample Descriptor</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t>OxfordNanopore_native</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Secondary Project</t>
   </si>
 </sst>
 </file>
@@ -2569,7 +2575,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F024D0-A71F-1D4F-B7B8-1935431836D0}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2578,113 +2584,125 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2695,19 +2713,19 @@
           <x14:formula1>
             <xm:f>faang_field_values!$C$3:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{8E8680DA-052A-464F-8853-7A707E219755}">
           <x14:formula1>
             <xm:f>faang_field_values!$C$2:$L$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D90F9425-0FCF-3F42-B5AD-EB00FB185850}">
           <x14:formula1>
             <xm:f>faang_field_values!$C$1:$N$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Removing hold until date from templates
</commit_message>
<xml_diff>
--- a/src/assets/atac-seq.xlsx
+++ b/src/assets/atac-seq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD579C-1CEF-B546-9FEA-1D214A7DD693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D5C326-67B5-9D4A-9910-6A3785C5C765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="277">
   <si>
     <t>Sample Descriptor</t>
   </si>
@@ -708,9 +708,6 @@
   </si>
   <si>
     <t>Alias</t>
-  </si>
-  <si>
-    <t>Hold Until Date</t>
   </si>
   <si>
     <t>Run center</t>
@@ -1256,9 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099D7B85-2870-7F44-9DA4-846DC9F871C9}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1270,9 +1265,7 @@
       <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>224</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1355,37 +1348,37 @@
         <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2577,7 +2570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F024D0-A71F-1D4F-B7B8-1935431836D0}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2621,10 +2614,10 @@
         <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -3416,131 +3409,131 @@
     </row>
     <row r="18" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" t="s">
         <v>237</v>
-      </c>
-      <c r="B18" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" t="s">
         <v>239</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>240</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>241</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>242</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>243</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>244</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>245</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>246</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>247</v>
-      </c>
-      <c r="J19" t="s">
-        <v>248</v>
       </c>
       <c r="K19" t="s">
         <v>72</v>
       </c>
       <c r="L19" t="s">
+        <v>248</v>
+      </c>
+      <c r="M19" t="s">
         <v>249</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>250</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>251</v>
-      </c>
-      <c r="O19" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" t="s">
         <v>253</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>254</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
         <v>255</v>
       </c>
-      <c r="D20" t="s">
-        <v>236</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>256</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>257</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>258</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>259</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>260</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>261</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>262</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>263</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>264</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>265</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>266</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>267</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>268</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>269</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>270</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>271</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>272</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>273</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>274</v>
-      </c>
-      <c r="X20" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>